<commit_message>
Addition of QA Script
</commit_message>
<xml_diff>
--- a/Record Export/generate_sql/Categorization Record Request.xlsx
+++ b/Record Export/generate_sql/Categorization Record Request.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnguyen\Desktop\Sandy York\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnguyen\Environmental Protection Agency (EPA)\ECMS - Documents\github\Document_Processing_Scripts\Record Export\generate_sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA0E91-5D19-4F0E-AF8A-AB8B68E06DE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{76FA0E91-5D19-4F0E-AF8A-AB8B68E06DE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{F5E0F8C2-3748-40D9-97D6-DDA204F84D10}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{974AFF44-CD47-46B7-923C-0AF2E484422D}"/>
+    <workbookView xWindow="1620" yWindow="1335" windowWidth="15105" windowHeight="13110" xr2:uid="{974AFF44-CD47-46B7-923C-0AF2E484422D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5684" uniqueCount="5386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5861" uniqueCount="5386">
   <si>
     <t>Organization</t>
   </si>
@@ -16580,10 +16580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98A77A42-8D92-451D-B94B-73FE2DE82643}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16606,758 +16606,983 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B2,Sheet2!A:B,2,FALSE),"")</f>
-        <v>LAND, CHEMICAL AND REDEVELOPMENT DIVISION</v>
+      <c r="A2" s="2" t="s">
+        <v>289</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5379</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>288</v>
+      </c>
+      <c r="C2" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B3,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="2" t="s">
+        <v>3078</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3077</v>
+      </c>
+      <c r="C3" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B4,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
+      <c r="A4" s="2" t="s">
+        <v>3066</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3065</v>
+      </c>
+      <c r="C4" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B5,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B6,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="2" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C6" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B7,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="2" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2081</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B8,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+      <c r="A8" s="2" t="s">
+        <v>2377</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2376</v>
+      </c>
+      <c r="C8" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B9,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B10,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B11,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C11" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B12,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="2" t="s">
+        <v>2382</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2381</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B13,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
+      <c r="A13" s="2" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C13" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B14,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
+      <c r="A14" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C14" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B15,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
+      <c r="A15" s="2" t="s">
+        <v>2417</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2416</v>
+      </c>
+      <c r="C15" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B16,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C16" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B17,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="C17" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B18,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C18" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B19,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="2" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C19" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B20,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="2" t="s">
+        <v>2380</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>2379</v>
+      </c>
+      <c r="C20" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B21,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C21" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B22,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
+      <c r="A22" s="2" t="s">
+        <v>2809</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2808</v>
+      </c>
+      <c r="C22" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B23,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B24,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B25,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
+      <c r="A25" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="C25" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B26,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C26" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B27,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
+      <c r="A27" s="2" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>2072</v>
+      </c>
+      <c r="C27" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B28,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
+      <c r="A28" s="2" t="s">
+        <v>2956</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2955</v>
+      </c>
+      <c r="C28" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B29,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
+      <c r="A29" s="2" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>3758</v>
+      </c>
+      <c r="C29" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B30,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
+      <c r="A30" s="2" t="s">
+        <v>2247</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>2246</v>
+      </c>
+      <c r="C30" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B31,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
+      <c r="A31" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C31" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B32,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
+      <c r="A32" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="C32" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B33,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
+      <c r="A33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B34,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
+      <c r="A34" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B35,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
+      <c r="A35" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="C35" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B36,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
+      <c r="A36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B37,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="3"/>
+      <c r="A37" s="2" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C37" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B38,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
+      <c r="A38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B39,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="3"/>
+      <c r="A39" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="C39" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B40,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="3"/>
+      <c r="A40" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B41,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="3"/>
+      <c r="A41" s="2" t="s">
+        <v>2428</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2427</v>
+      </c>
+      <c r="C41" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B42,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
+      <c r="A42" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B43,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="3"/>
+      <c r="A43" s="2" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C43" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B44,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="3"/>
+      <c r="A44" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C44" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B45,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="3"/>
+      <c r="A45" s="2" t="s">
+        <v>2956</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B46,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="3"/>
+      <c r="A46" s="2" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>2335</v>
+      </c>
+      <c r="C46" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B47,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="3"/>
+      <c r="A47" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="C47" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B48,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="3"/>
+      <c r="A48" s="2" t="s">
+        <v>2569</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>2568</v>
+      </c>
+      <c r="C48" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B49,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="3"/>
+      <c r="A49" s="2" t="s">
+        <v>2589</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>2588</v>
+      </c>
+      <c r="C49" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B50,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="3"/>
+      <c r="A50" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="C50" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B51,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="3"/>
+      <c r="A51" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C51" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B52,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="3"/>
+      <c r="A52" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="C52" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B53,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="3"/>
+      <c r="A53" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B54,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="3"/>
+      <c r="A54" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C54" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B55,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="3"/>
+      <c r="A55" s="2" t="s">
+        <v>4543</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>4542</v>
+      </c>
+      <c r="C55" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B56,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="3"/>
+      <c r="A56" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="C56" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B57,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="3"/>
+      <c r="A57" s="2" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C57" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B58,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="3"/>
+      <c r="A58" s="2" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C58" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B59,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="3"/>
+      <c r="A59" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C59" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B60,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B60" s="2"/>
-      <c r="C60" s="3"/>
+      <c r="A60" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C60" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B61,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="3"/>
+      <c r="A61" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>3218</v>
+      </c>
+      <c r="C61" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B62,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="3"/>
+      <c r="A62" s="2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C62" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B63,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="3"/>
+      <c r="A63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B64,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="3"/>
+      <c r="A64" s="2" t="s">
+        <v>3230</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>3229</v>
+      </c>
+      <c r="C64" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B65,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="3"/>
+      <c r="A65" s="2" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>3319</v>
+      </c>
+      <c r="C65" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B66,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="3"/>
+      <c r="A66" s="2" t="s">
+        <v>2131</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>2130</v>
+      </c>
+      <c r="C66" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B67,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="3"/>
+      <c r="A67" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C67" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B68,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="3"/>
+      <c r="A68" s="2" t="s">
+        <v>2595</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>2594</v>
+      </c>
+      <c r="C68" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B69,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B69" s="2"/>
-      <c r="C69" s="3"/>
+      <c r="A69" s="2" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>2009</v>
+      </c>
+      <c r="C69" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B70,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="3"/>
+      <c r="A70" s="2" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C70" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B71,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="3"/>
+      <c r="A71" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C71" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B72,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="3"/>
+      <c r="A72" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C72" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B73,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="3"/>
+      <c r="A73" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="C73" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B74,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" s="3"/>
+      <c r="A74" s="2" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C74" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B75,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="3"/>
+      <c r="A75" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>2145</v>
+      </c>
+      <c r="C75" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B76,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="3"/>
+      <c r="A76" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C76" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B77,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B77" s="2"/>
-      <c r="C77" s="3"/>
+      <c r="A77" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C77" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B78,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B78" s="2"/>
-      <c r="C78" s="3"/>
+      <c r="A78" s="2" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C78" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B79,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B79" s="2"/>
-      <c r="C79" s="3"/>
+      <c r="A79" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>2793</v>
+      </c>
+      <c r="C79" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B80,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="3"/>
+      <c r="A80" s="2" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>2793</v>
+      </c>
+      <c r="C80" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B81,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="3"/>
+      <c r="A81" s="2" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C81" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B82,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B82" s="2"/>
-      <c r="C82" s="3"/>
+      <c r="A82" s="2" t="s">
+        <v>2852</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>2851</v>
+      </c>
+      <c r="C82" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B83,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B83" s="2"/>
-      <c r="C83" s="3"/>
+      <c r="A83" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>3251</v>
+      </c>
+      <c r="C83" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B84,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B84" s="2"/>
-      <c r="C84" s="3"/>
+      <c r="A84" s="2" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>3247</v>
+      </c>
+      <c r="C84" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B85,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B85" s="2"/>
-      <c r="C85" s="3"/>
+      <c r="A85" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C85" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B86,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B86" s="2"/>
-      <c r="C86" s="3"/>
+      <c r="A86" s="2" t="s">
+        <v>966</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="C86" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B87,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="3"/>
+      <c r="A87" s="2" t="s">
+        <v>3189</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>3188</v>
+      </c>
+      <c r="C87" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B88,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B88" s="2"/>
-      <c r="C88" s="3"/>
+      <c r="A88" s="2" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C88" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B89,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B89" s="2"/>
-      <c r="C89" s="3"/>
+      <c r="A89" s="2" t="s">
+        <v>5101</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>5100</v>
+      </c>
+      <c r="C89" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B90,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B90" s="2"/>
-      <c r="C90" s="3"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B91,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B92,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B93,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B94,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="str">
-        <f>IFERROR(VLOOKUP(B95,Sheet2!A:B,2,FALSE),"")</f>
-        <v/>
-      </c>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
+      <c r="A90" s="2" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>4839</v>
+      </c>
+      <c r="C90" s="3">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17368,7 +17593,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B95</xm:sqref>
+          <xm:sqref>B2:B90</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -40593,17 +40818,53 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD48CB8A-1B8B-4207-BACF-A6AA8DE61C41}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD48CB8A-1B8B-4207-BACF-A6AA8DE61C41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="18efe1b8-b951-4c9f-8f49-5286143281c8"/>
+    <ds:schemaRef ds:uri="71ac8f93-32f7-41cd-b35d-e5524536188c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ADC5A16-864D-48E3-9DAE-2C4A24197FCA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ADC5A16-864D-48E3-9DAE-2C4A24197FCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45EE8EFA-820A-48FC-BDFA-A01CD8FD334B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45EE8EFA-820A-48FC-BDFA-A01CD8FD334B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8E54E3D-0A20-4ECA-8F51-30FCA99AD555}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8E54E3D-0A20-4ECA-8F51-30FCA99AD555}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>